<commit_message>
added markets, improved spawn choices, and moved winning calculations to host tick
</commit_message>
<xml_diff>
--- a/resources.xlsx
+++ b/resources.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benthomas/Sites/firebase-test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD75619-8781-9940-A580-E0FBB95D1492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780411E1-03D9-6F40-9D2B-A69AA1B6F3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6580" yWindow="18380" windowWidth="22160" windowHeight="15140" xr2:uid="{EB3F0EE2-A324-5340-B28F-ADDB9AD620F3}"/>
+    <workbookView xWindow="6580" yWindow="16620" windowWidth="22160" windowHeight="15140" xr2:uid="{EB3F0EE2-A324-5340-B28F-ADDB9AD620F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>biomes:</t>
   </si>
@@ -148,6 +148,21 @@
   </si>
   <si>
     <t>charge any time a new unit is recruited?</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>black</t>
   </si>
 </sst>
 </file>
@@ -514,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABA86AAA-B40E-9141-B3FF-0F15A4FFD31D}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,7 +540,7 @@
     <col min="1" max="1" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>10</v>
@@ -546,7 +561,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -556,7 +571,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -585,8 +600,11 @@
       <c r="I3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -612,8 +630,11 @@
       <c r="H4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -639,8 +660,11 @@
       <c r="H5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -663,8 +687,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -687,8 +714,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2">
         <f>SUM(B3:B7)</f>
@@ -711,7 +741,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -719,7 +749,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -727,7 +757,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -735,7 +765,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -743,7 +773,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -751,7 +781,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -759,7 +789,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -767,7 +797,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>

</xml_diff>